<commit_message>
Added a graph showing improvements to software
</commit_message>
<xml_diff>
--- a/Lmpsdata.xlsx
+++ b/Lmpsdata.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16820" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16820" windowHeight="16620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -73,6 +73,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -349,37 +350,75 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2118254360"/>
-        <c:axId val="-2118409448"/>
+        <c:axId val="2135481032"/>
+        <c:axId val="2135484024"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2118254360"/>
+        <c:axId val="2135481032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number of atoms</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118409448"/>
+        <c:crossAx val="2135484024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2118409448"/>
+        <c:axId val="2135484024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" vert="wordArtVert"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Minutes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2118254360"/>
+        <c:crossAx val="2135481032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -761,7 +800,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>